<commit_message>
Atualização automática de TORRES.xlsx
</commit_message>
<xml_diff>
--- a/TORRES.xlsx
+++ b/TORRES.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92419533-DFBE-43DE-A92A-248E8E17276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D30F613-ACAC-4CC0-AEA5-2A1490678FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="7" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="8" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
     <sheet name="CPIP" sheetId="4" r:id="rId5"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
+    <sheet name="DGC" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="318">
   <si>
     <t>COMARCA</t>
   </si>
@@ -968,6 +969,18 @@
   </si>
   <si>
     <t>TORRES</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MOT-VIG</t>
+  </si>
+  <si>
+    <t>Validou posto que não existe na comarca</t>
   </si>
 </sst>
 </file>
@@ -977,7 +990,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1030,6 +1043,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1044,7 +1070,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1085,6 +1111,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1157,9 +1189,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1241,12 +1273,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{BCCA4904-0582-478D-8E32-779DF7B8A219}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{550706B9-2F33-4134-930D-F4B38580DD24}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1276,10 +1312,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA14710-1365-4F27-AB63-31BFF64E65F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4DD56B0-CC67-49BC-B84A-FBC2F68DF874}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1317,7 +1353,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD02631-1A42-443C-BC6A-09E0DF329F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAE8C135-C26F-4DAA-99B4-6AD9394D457F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1380,7 +1416,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92CF7DD-1AAA-4A81-91B9-DF93B94B867B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{988B3A00-9369-4B60-80F9-19D5A1AA8B46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1399,7 +1435,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BC94C1-E700-6043-9D87-1A9147B64B29}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E404F2C-3186-6AB6-EA7F-D446088988CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1448,7 +1484,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F196B04F-E8C1-F064-F04D-02C538DAA50A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877680C1-CC16-94CD-F4FB-46EBC3F69B9E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1467,7 +1503,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4265EBF3-CAF6-083B-8BE0-3DA0331B0467}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC317FD3-CDCC-608A-C567-E2D7A3E47546}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1498,7 +1534,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC1BA28-82DA-AB55-A4A3-CF0ABCA8DF7E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E8B8F00-D104-AD3A-3059-EC2F11DBB4BB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1529,7 +1565,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325572EF-C8F5-C5D6-44A4-0C62EF8FD970}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F065F80-5188-08A0-6C85-D47D9EC76ABC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1572,7 +1608,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675EA388-E9E0-4A75-88BB-2559C23EBC30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9DC015-0BFB-4F93-8423-669BAB4EA570}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1610,7 +1646,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687553F0-FDCA-49B1-9860-99F5BD081B2F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963E691B-1D21-41B9-B776-B1948CD6E550}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1653,7 +1689,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D9EDC11-ACB5-4FE4-AD34-AA35A522F965}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5D423BF-B3AE-4F68-9A1C-9E265A2FDCF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1966,7 +2002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047A66D8-2817-487E-9F41-2DF336BD0E56}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B650FC-FF07-47AB-AEB7-4BFEC080D85F}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1978,98 +2014,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="34"/>
-    <col min="6" max="6" width="2" style="34" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="34"/>
+    <col min="1" max="5" width="12.5703125" style="36"/>
+    <col min="6" max="6" width="2" style="36" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="33"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="33"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="33"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="33"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="33"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="33"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="33"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="33"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="33"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="33"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="33"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="33"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="33"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="33"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="33"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="33"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="33"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="33"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="33"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="33"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="33"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="33"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="33"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="33"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="33"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="33"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="33"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5736,4 +5772,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>